<commit_message>
failed attempt for inserting futures contract
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="2" r:id="rId1"/>
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Account Info</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Mode</t>
+  </si>
+  <si>
+    <t>Total Exposure</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1114,6 +1117,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1138,30 +1165,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -1218,6 +1224,841 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Exposure to Equity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1A28-4BAE-BC6E-8DD09BD92C09}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1A28-4BAE-BC6E-8DD09BD92C09}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Portfolio!$A$5,Portfolio!$A$12)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Equity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total Exposure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Portfolio!$B$5,Portfolio!$B$12)</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1030.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A28-4BAE-BC6E-8DD09BD92C09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="75"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1486,15 +2327,15 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1582,6 +2423,15 @@
       </c>
       <c r="B11" s="56">
         <f>B10/B9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="57">
+        <f>SUM(Positions!H11:H30)</f>
         <v>0</v>
       </c>
     </row>
@@ -1595,6 +2445,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1605,8 +2456,8 @@
   </sheetPr>
   <dimension ref="D8:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,22 +2485,22 @@
   <sheetData>
     <row r="8" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="94" t="s">
+      <c r="K9" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="95"/>
-      <c r="M9" s="96" t="s">
+      <c r="L9" s="87"/>
+      <c r="M9" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="97"/>
-      <c r="Q9" s="98" t="s">
+      <c r="N9" s="89"/>
+      <c r="Q9" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="R9" s="99"/>
-      <c r="S9" s="100" t="s">
+      <c r="R9" s="91"/>
+      <c r="S9" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="T9" s="101"/>
+      <c r="T9" s="93"/>
     </row>
     <row r="10" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="12" t="s">
@@ -1712,7 +2563,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="28"/>
       <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
+      <c r="H11" s="102"/>
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
       <c r="K11" s="48"/>
@@ -1732,7 +2583,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="3"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="103"/>
       <c r="I12" s="4"/>
       <c r="J12" s="25"/>
       <c r="K12" s="49"/>
@@ -1752,7 +2603,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="3"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="103"/>
       <c r="I13" s="4"/>
       <c r="J13" s="22"/>
       <c r="K13" s="49"/>
@@ -1772,7 +2623,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="3"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="103"/>
       <c r="I14" s="4"/>
       <c r="J14" s="22"/>
       <c r="K14" s="49"/>
@@ -1792,7 +2643,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="3"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="103"/>
       <c r="I15" s="4"/>
       <c r="J15" s="22"/>
       <c r="K15" s="49"/>
@@ -1812,7 +2663,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="103"/>
       <c r="I16" s="4"/>
       <c r="J16" s="22"/>
       <c r="K16" s="49"/>
@@ -1832,7 +2683,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="3"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="103"/>
       <c r="I17" s="4"/>
       <c r="J17" s="22"/>
       <c r="K17" s="49"/>
@@ -1852,7 +2703,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="3"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="103"/>
       <c r="I18" s="4"/>
       <c r="J18" s="22"/>
       <c r="K18" s="49"/>
@@ -1872,7 +2723,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="3"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="103"/>
       <c r="I19" s="4"/>
       <c r="J19" s="22"/>
       <c r="K19" s="49"/>
@@ -1892,7 +2743,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="103"/>
       <c r="I20" s="4"/>
       <c r="J20" s="22"/>
       <c r="K20" s="49"/>
@@ -1912,7 +2763,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="3"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="103"/>
       <c r="I21" s="4"/>
       <c r="J21" s="22"/>
       <c r="K21" s="49"/>
@@ -1932,7 +2783,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="3"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="103"/>
       <c r="I22" s="4"/>
       <c r="J22" s="22"/>
       <c r="K22" s="49"/>
@@ -1952,7 +2803,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="3"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="4"/>
+      <c r="H23" s="103"/>
       <c r="I23" s="4"/>
       <c r="J23" s="22"/>
       <c r="K23" s="49"/>
@@ -1972,7 +2823,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="3"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="103"/>
       <c r="I24" s="4"/>
       <c r="J24" s="22"/>
       <c r="K24" s="49"/>
@@ -1992,7 +2843,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="3"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="103"/>
       <c r="I25" s="4"/>
       <c r="J25" s="22"/>
       <c r="K25" s="49"/>
@@ -2012,7 +2863,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="3"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="4"/>
+      <c r="H26" s="103"/>
       <c r="I26" s="4"/>
       <c r="J26" s="22"/>
       <c r="K26" s="49"/>
@@ -2032,7 +2883,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="3"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="103"/>
       <c r="I27" s="4"/>
       <c r="J27" s="22"/>
       <c r="K27" s="49"/>
@@ -2052,7 +2903,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="3"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="103"/>
       <c r="I28" s="4"/>
       <c r="J28" s="22"/>
       <c r="K28" s="49"/>
@@ -2072,7 +2923,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="3"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="103"/>
       <c r="I29" s="4"/>
       <c r="J29" s="22"/>
       <c r="K29" s="49"/>
@@ -2092,7 +2943,7 @@
       <c r="E30" s="41"/>
       <c r="F30" s="42"/>
       <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="H30" s="104"/>
       <c r="I30" s="44"/>
       <c r="J30" s="45"/>
       <c r="K30" s="50"/>
@@ -2212,22 +3063,22 @@
   <sheetData>
     <row r="8" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J9" s="86" t="s">
+      <c r="J9" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="87"/>
-      <c r="L9" s="88" t="s">
+      <c r="K9" s="95"/>
+      <c r="L9" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="89"/>
-      <c r="N9" s="90" t="s">
+      <c r="M9" s="97"/>
+      <c r="N9" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="91"/>
-      <c r="P9" s="92" t="s">
+      <c r="O9" s="99"/>
+      <c r="P9" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="93"/>
+      <c r="Q9" s="101"/>
     </row>
     <row r="10" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="12" t="s">

</xml_diff>